<commit_message>
Uploaded 22-Oct-2021 17:27:06 {/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx
+++ b/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\212810063\Documents\DTLP\Rotation 1\Drools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8060103-CA9B-4806-A7B3-31BFABF0A746}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A2EE9C-D2FA-403D-B87D-930709587A3F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7981FC14-C66D-4D3E-979A-738784BB6AA4}"/>
+    <workbookView xWindow="2100" yWindow="100" windowWidth="15510" windowHeight="9590" xr2:uid="{7981FC14-C66D-4D3E-979A-738784BB6AA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,12 +39,6 @@
     <t>RuleSet</t>
   </si>
   <si>
-    <t>RuleTable InvestorApproval</t>
-  </si>
-  <si>
-    <t>Investor Approval</t>
-  </si>
-  <si>
     <t>object type (optional)</t>
   </si>
   <si>
@@ -103,6 +97,12 @@
   </si>
   <si>
     <t>autogen == $param</t>
+  </si>
+  <si>
+    <t>Auto Doc Gen</t>
+  </si>
+  <si>
+    <t>RuleTable AutoDocGen</t>
   </si>
 </sst>
 </file>
@@ -196,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -205,14 +205,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -527,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31998A4C-F8CB-4948-91B9-76A28CCA9776}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -543,131 +544,137 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="2"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
-      <c r="B4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="6" t="s">
+      <c r="B4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="3"/>
+      <c r="B5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>6</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="10" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="E7" s="6"/>
+      <c r="F7" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="C8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="12" t="s">
+      <c r="D8" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C9" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13" t="s">
+      <c r="D9" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="E9" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="13" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13" t="s">
+      <c r="D10" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="13" t="b">
+      <c r="E10" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="12" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Uploaded 22-Oct-2021 17:27:40 {/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx
+++ b/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\212810063\Documents\DTLP\Rotation 1\Drools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A2EE9C-D2FA-403D-B87D-930709587A3F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792B4A9C-23BC-4EB1-8F22-718B32B48AB0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2100" yWindow="100" windowWidth="15510" windowHeight="9590" xr2:uid="{7981FC14-C66D-4D3E-979A-738784BB6AA4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>RuleSet</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>it may contain textual descriptions of the column's purpose (ignored)</t>
-  </si>
-  <si>
-    <t>autodocgen</t>
   </si>
   <si>
     <t>$document: Document</t>
@@ -531,7 +528,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -550,7 +547,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1"/>
     </row>
@@ -563,7 +560,7 @@
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -593,13 +590,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
       <c r="E6" s="8"/>
       <c r="F6" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -607,17 +604,17 @@
         <v>2</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>11</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>12</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -625,13 +622,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>14</v>
-      </c>
       <c r="D8" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
@@ -639,16 +636,16 @@
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="12"/>
       <c r="B9" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="D9" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>17</v>
-      </c>
       <c r="E9" s="12" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="F9" s="12" t="b">
         <v>1</v>
@@ -657,16 +654,16 @@
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="12"/>
       <c r="B10" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="F10" s="12" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Uploaded 22-Oct-2021 17:34:36 {/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx
+++ b/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\212810063\Documents\DTLP\Rotation 1\Drools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792B4A9C-23BC-4EB1-8F22-718B32B48AB0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A71521-AFE4-490F-A063-2C1A08D7346C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2100" yWindow="100" windowWidth="15510" windowHeight="9590" xr2:uid="{7981FC14-C66D-4D3E-979A-738784BB6AA4}"/>
   </bookViews>
@@ -93,13 +93,13 @@
     <t>$document</t>
   </si>
   <si>
-    <t>autogen == $param</t>
-  </si>
-  <si>
     <t>Auto Doc Gen</t>
   </si>
   <si>
     <t>RuleTable AutoDocGen</t>
+  </si>
+  <si>
+    <t>autogen = $param</t>
   </si>
 </sst>
 </file>
@@ -528,7 +528,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -547,7 +547,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1"/>
     </row>
@@ -560,7 +560,7 @@
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -614,7 +614,7 @@
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -645,7 +645,7 @@
         <v>16</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F9" s="12" t="b">
         <v>1</v>
@@ -663,7 +663,7 @@
         <v>16</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F10" s="12" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Uploaded 22-Oct-2021 17:44:13 {/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx
+++ b/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\212810063\Documents\DTLP\Rotation 1\Drools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A71521-AFE4-490F-A063-2C1A08D7346C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C5ECFAA-9629-46B7-843B-9CFA9DCB1823}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2100" yWindow="100" windowWidth="15510" windowHeight="9590" xr2:uid="{7981FC14-C66D-4D3E-979A-738784BB6AA4}"/>
   </bookViews>
@@ -99,7 +99,7 @@
     <t>RuleTable AutoDocGen</t>
   </si>
   <si>
-    <t>autogen = $param</t>
+    <t>autogen</t>
   </si>
 </sst>
 </file>
@@ -528,7 +528,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Uploaded 22-Oct-2021 17:46:15 {/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx
+++ b/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\212810063\Documents\DTLP\Rotation 1\Drools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C5ECFAA-9629-46B7-843B-9CFA9DCB1823}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250FB45B-A5D7-4ED8-8CEE-17AF8245F307}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2100" yWindow="100" windowWidth="15510" windowHeight="9590" xr2:uid="{7981FC14-C66D-4D3E-979A-738784BB6AA4}"/>
   </bookViews>
@@ -93,13 +93,13 @@
     <t>$document</t>
   </si>
   <si>
+    <t>autogen == $param</t>
+  </si>
+  <si>
     <t>Auto Doc Gen</t>
   </si>
   <si>
     <t>RuleTable AutoDocGen</t>
-  </si>
-  <si>
-    <t>autogen</t>
   </si>
 </sst>
 </file>
@@ -528,7 +528,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -547,7 +547,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1"/>
     </row>
@@ -560,7 +560,7 @@
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -614,7 +614,7 @@
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -645,7 +645,7 @@
         <v>16</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F9" s="12" t="b">
         <v>1</v>
@@ -663,7 +663,7 @@
         <v>16</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F10" s="12" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Uploaded 22-Oct-2021 17:57:50 {/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx
+++ b/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\212810063\Documents\DTLP\Rotation 1\Drools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250FB45B-A5D7-4ED8-8CEE-17AF8245F307}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E322FA-AFA7-4834-BD7D-51F52A4171B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="100" windowWidth="15510" windowHeight="9590" xr2:uid="{7981FC14-C66D-4D3E-979A-738784BB6AA4}"/>
+    <workbookView xWindow="2750" yWindow="2100" windowWidth="15510" windowHeight="9590" xr2:uid="{7981FC14-C66D-4D3E-979A-738784BB6AA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>RuleSet</t>
   </si>
@@ -93,13 +93,19 @@
     <t>$document</t>
   </si>
   <si>
-    <t>autogen == $param</t>
-  </si>
-  <si>
     <t>Auto Doc Gen</t>
   </si>
   <si>
     <t>RuleTable AutoDocGen</t>
+  </si>
+  <si>
+    <t>Import</t>
+  </si>
+  <si>
+    <t>com.myspace.eotworkflow.*</t>
+  </si>
+  <si>
+    <t>document.setAutogen($param)</t>
   </si>
 </sst>
 </file>
@@ -528,7 +534,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -536,7 +542,7 @@
     <col min="1" max="1" width="58.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="24.453125" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="18.1796875" customWidth="1"/>
+    <col min="6" max="6" width="29.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -547,20 +553,24 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
+      <c r="B2" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
       <c r="D2" s="14"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -614,7 +624,7 @@
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="7" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -645,7 +655,7 @@
         <v>16</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F9" s="12" t="b">
         <v>1</v>
@@ -663,7 +673,7 @@
         <v>16</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F10" s="12" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Uploaded 22-Oct-2021 17:59:05 {/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx
+++ b/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\212810063\Documents\DTLP\Rotation 1\Drools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E322FA-AFA7-4834-BD7D-51F52A4171B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE55D3D6-077D-4B01-8E01-716EBAEA04AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2750" yWindow="2100" windowWidth="15510" windowHeight="9590" xr2:uid="{7981FC14-C66D-4D3E-979A-738784BB6AA4}"/>
   </bookViews>
@@ -60,9 +60,6 @@
     <t>it may contain textual descriptions of the column's purpose (ignored)</t>
   </si>
   <si>
-    <t>$document: Document</t>
-  </si>
-  <si>
     <t>relationshipname</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
     <t>Bill of Sale</t>
   </si>
   <si>
-    <t>$document</t>
-  </si>
-  <si>
     <t>Auto Doc Gen</t>
   </si>
   <si>
@@ -106,6 +100,12 @@
   </si>
   <si>
     <t>document.setAutogen($param)</t>
+  </si>
+  <si>
+    <t>document: Document</t>
+  </si>
+  <si>
+    <t>document</t>
   </si>
 </sst>
 </file>
@@ -534,7 +534,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -553,24 +553,24 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D2" s="14"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -600,13 +600,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
       <c r="E6" s="8"/>
       <c r="F6" s="9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -614,17 +614,17 @@
         <v>2</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>11</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -632,13 +632,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>13</v>
-      </c>
       <c r="D8" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
@@ -646,16 +646,16 @@
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="12"/>
       <c r="B9" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="D9" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>16</v>
-      </c>
       <c r="E9" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F9" s="12" t="b">
         <v>1</v>
@@ -664,16 +664,16 @@
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="12"/>
       <c r="B10" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="12" t="s">
         <v>17</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>19</v>
       </c>
       <c r="F10" s="12" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Uploaded 22-Oct-2021 18:00:32 {/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx
+++ b/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\212810063\Documents\DTLP\Rotation 1\Drools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE55D3D6-077D-4B01-8E01-716EBAEA04AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C576FED-A43C-40AB-BBA4-7EDC341FBF1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2750" yWindow="2100" windowWidth="15510" windowHeight="9590" xr2:uid="{7981FC14-C66D-4D3E-979A-738784BB6AA4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>RuleSet</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>document: Document</t>
-  </si>
-  <si>
-    <t>document</t>
   </si>
 </sst>
 </file>
@@ -534,7 +531,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -605,9 +602,7 @@
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="9" t="s">
-        <v>23</v>
-      </c>
+      <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">

</xml_diff>

<commit_message>
Uploaded 22-Oct-2021 18:01:35 {/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx
+++ b/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\212810063\Documents\DTLP\Rotation 1\Drools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C576FED-A43C-40AB-BBA4-7EDC341FBF1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C92B21C-E920-428B-8B6C-D979F69B9C41}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2750" yWindow="2100" windowWidth="15510" windowHeight="9590" xr2:uid="{7981FC14-C66D-4D3E-979A-738784BB6AA4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>RuleSet</t>
   </si>
@@ -96,13 +96,16 @@
     <t>Import</t>
   </si>
   <si>
+    <t>com.myspace.eotworkflow</t>
+  </si>
+  <si>
     <t>com.myspace.eotworkflow.*</t>
   </si>
   <si>
-    <t>document.setAutogen($param)</t>
-  </si>
-  <si>
     <t>document: Document</t>
+  </si>
+  <si>
+    <t>document.setAutogen($1)</t>
   </si>
 </sst>
 </file>
@@ -531,7 +534,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -549,8 +552,8 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>17</v>
+      <c r="C1" t="s">
+        <v>20</v>
       </c>
       <c r="D1" s="1"/>
     </row>
@@ -560,7 +563,7 @@
         <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2" s="14"/>
     </row>
@@ -619,7 +622,7 @@
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Uploaded 22-Oct-2021 18:02:21 {/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx
+++ b/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\212810063\Documents\DTLP\Rotation 1\Drools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C92B21C-E920-428B-8B6C-D979F69B9C41}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5495161-F4AC-4481-A284-0C1023064BCF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2750" yWindow="2100" windowWidth="15510" windowHeight="9590" xr2:uid="{7981FC14-C66D-4D3E-979A-738784BB6AA4}"/>
   </bookViews>
@@ -105,7 +105,7 @@
     <t>document: Document</t>
   </si>
   <si>
-    <t>document.setAutogen($1)</t>
+    <t>document.setAutogen($1);</t>
   </si>
 </sst>
 </file>
@@ -534,7 +534,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Uploaded 22-Oct-2021 18:05:17 {/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx
+++ b/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\212810063\Documents\DTLP\Rotation 1\Drools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5495161-F4AC-4481-A284-0C1023064BCF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0EC5F8D-F2A3-4CE6-B252-0E8D21E7D0AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2750" yWindow="2100" windowWidth="15510" windowHeight="9590" xr2:uid="{7981FC14-C66D-4D3E-979A-738784BB6AA4}"/>
   </bookViews>
@@ -60,6 +60,9 @@
     <t>it may contain textual descriptions of the column's purpose (ignored)</t>
   </si>
   <si>
+    <t>$document: Document</t>
+  </si>
+  <si>
     <t>relationshipname</t>
   </si>
   <si>
@@ -102,10 +105,7 @@
     <t>com.myspace.eotworkflow.*</t>
   </si>
   <si>
-    <t>document: Document</t>
-  </si>
-  <si>
-    <t>document.setAutogen($1);</t>
+    <t>$document.setAutogen($1);</t>
   </si>
 </sst>
 </file>
@@ -553,24 +553,24 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D2" s="14"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -600,7 +600,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
@@ -612,13 +612,13 @@
         <v>2</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="7" t="s">
@@ -630,13 +630,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>11</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>10</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
@@ -644,16 +644,16 @@
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="12"/>
       <c r="B9" s="12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F9" s="12" t="b">
         <v>1</v>
@@ -662,16 +662,16 @@
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="12"/>
       <c r="B10" s="12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="12" t="s">
-        <v>15</v>
-      </c>
       <c r="E10" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F10" s="12" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Uploaded 22-Oct-2021 19:48:45 {/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx
+++ b/src/main/resources/com/myspace/eotworkflow/Auto Doc Gen Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\212810063\Documents\DTLP\Rotation 1\Drools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0EC5F8D-F2A3-4CE6-B252-0E8D21E7D0AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B9FCEE-106B-4964-8B18-2B024FC7B0E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2750" yWindow="2100" windowWidth="15510" windowHeight="9590" xr2:uid="{7981FC14-C66D-4D3E-979A-738784BB6AA4}"/>
+    <workbookView xWindow="4440" yWindow="3860" windowWidth="15510" windowHeight="9590" xr2:uid="{7981FC14-C66D-4D3E-979A-738784BB6AA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>RuleSet</t>
   </si>
@@ -60,9 +60,6 @@
     <t>it may contain textual descriptions of the column's purpose (ignored)</t>
   </si>
   <si>
-    <t>$document: Document</t>
-  </si>
-  <si>
     <t>relationshipname</t>
   </si>
   <si>
@@ -105,14 +102,23 @@
     <t>com.myspace.eotworkflow.*</t>
   </si>
   <si>
-    <t>$document.setAutogen($1);</t>
+    <t>document: Document</t>
+  </si>
+  <si>
+    <t>Declare</t>
+  </si>
+  <si>
+    <t>dialect "mvel";</t>
+  </si>
+  <si>
+    <t>document.setAutogen($param);</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,6 +132,10 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="8">
@@ -196,10 +206,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -217,9 +228,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{5EB34667-10E4-47A9-B9AB-F01C8BFFD64A}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -553,24 +566,32 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="14"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B3" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -600,7 +621,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
@@ -612,17 +633,17 @@
         <v>2</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>11</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -630,13 +651,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>13</v>
-      </c>
       <c r="D8" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
@@ -644,16 +665,16 @@
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="12"/>
       <c r="B9" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="D9" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>16</v>
-      </c>
       <c r="E9" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F9" s="12" t="b">
         <v>1</v>
@@ -662,16 +683,16 @@
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="12"/>
       <c r="B10" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="12" t="s">
         <v>17</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>18</v>
       </c>
       <c r="F10" s="12" t="b">
         <v>1</v>

</xml_diff>